<commit_message>
bissl was bei der banf geändert
</commit_message>
<xml_diff>
--- a/Ressourcen/mitarbeiterExcel.xlsx
+++ b/Ressourcen/mitarbeiterExcel.xlsx
@@ -3,9 +3,9 @@
 <x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <x:fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{680464C9-F93B-4874-AC88-CE19C37375B2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{780BB0EF-C075-456D-8FF6-D7514B7EB000}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <x:bookViews>
-    <x:workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <x:si>
     <x:t>Anrede</x:t>
   </x:si>
@@ -74,15 +74,91 @@
     <x:t>Lohnsteuerklasse</x:t>
   </x:si>
   <x:si>
-    <x:t>SAP Nutzer</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Business Partner</x:t>
+    <x:t>SAP Benutzer?</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Business Partner?</x:t>
   </x:si>
   <x:si>
     <x:t>Equipment</x:t>
   </x:si>
   <x:si>
+    <x:t xml:space="preserve">Frau 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Holle 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Angelika 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">03.03.1985 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Helwink 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">5 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">52132 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Bern 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Angelika.Holle@ap-solut.com 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">92312312321 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Sparkasse Helwink 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">WELAD3DLE 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3123121233 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">221122 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">05.05.2015 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Vertrieb 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">2 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Ja 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">MacBook 
+</x:t>
+  </x:si>
+  <x:si>
     <x:t xml:space="preserve">Herr 
 </x:t>
   </x:si>
@@ -155,7 +231,63 @@
 </x:t>
   </x:si>
   <x:si>
-    <x:t xml:space="preserve">MacBook 
+    <x:t xml:space="preserve">Mustermann 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Max 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">12.12.1990 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Musterstrasse 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">33566 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Musterstadt 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Max.Mustermann@ap-solut.com 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">38921083 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Volksbank Lübbecker Land eG 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">GENODEM1LUB 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">431431 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">43143143 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">12.12.2012 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">Reinigungskraft 
+</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">1 
 </x:t>
   </x:si>
 </x:sst>
@@ -206,54 +338,12 @@
       <x:diagonal/>
     </x:border>
   </x:borders>
-  <x:cellStyleXfs count="23">
+  <x:cellStyleXfs count="9">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
     <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -277,10 +367,10 @@
   </x:cellStyleXfs>
   <x:cellXfs count="8">
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment wrapText="1"/>
     </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <x:alignment wrapText="1"/>
     </x:xf>
@@ -288,12 +378,12 @@
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
     <x:xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
       <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <x:protection locked="1" hidden="0"/>
-    </x:xf>
-    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
-      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <x:protection locked="1" hidden="0"/>
     </x:xf>
     <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
@@ -585,262 +675,324 @@
   <x:dimension ref="A1:T12"/>
   <x:sheetViews>
     <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A6" sqref="A6 A6:A6 A1:XFD1048576"/>
+      <x:selection activeCell="C16" sqref="C16 C16:C16"/>
     </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr baseColWidth="10" defaultColWidth="57.676563" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetFormatPr baseColWidth="10" defaultColWidth="27.702188" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
     <x:row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A1" s="6" t="s">
+      <x:c r="A1" s="5" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="6" t="s">
+      <x:c r="B1" s="5" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="6" t="s">
+      <x:c r="C1" s="5" t="s">
         <x:v>2</x:v>
       </x:c>
-      <x:c r="D1" s="6" t="s">
+      <x:c r="D1" s="5" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="E1" s="6" t="s">
+      <x:c r="E1" s="5" t="s">
         <x:v>4</x:v>
       </x:c>
-      <x:c r="F1" s="6" t="s">
+      <x:c r="F1" s="5" t="s">
         <x:v>5</x:v>
       </x:c>
-      <x:c r="G1" s="6" t="s">
+      <x:c r="G1" s="5" t="s">
         <x:v>6</x:v>
       </x:c>
-      <x:c r="H1" s="6" t="s">
+      <x:c r="H1" s="5" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="I1" s="6" t="s">
+      <x:c r="I1" s="5" t="s">
         <x:v>8</x:v>
       </x:c>
-      <x:c r="J1" s="6" t="s">
+      <x:c r="J1" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="6" t="s">
+      <x:c r="K1" s="5" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="6" t="s">
+      <x:c r="L1" s="5" t="s">
         <x:v>11</x:v>
       </x:c>
-      <x:c r="M1" s="6" t="s">
+      <x:c r="M1" s="5" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="N1" s="6" t="s">
+      <x:c r="N1" s="5" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="O1" s="6" t="s">
+      <x:c r="O1" s="5" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="P1" s="6" t="s">
+      <x:c r="P1" s="5" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="Q1" s="6" t="s">
+      <x:c r="Q1" s="5" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="R1" s="6" t="s">
+      <x:c r="R1" s="5" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="S1" s="6" t="s">
+      <x:c r="S1" s="5" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="T1" s="6" t="s">
+      <x:c r="T1" s="5" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A2" s="5" t="s">
+      <x:c r="A2" s="6" t="s">
         <x:v>20</x:v>
       </x:c>
       <x:c r="B2" s="7" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="C2" s="5" t="s">
+      <x:c r="C2" s="6" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="D2" s="5" t="s">
+      <x:c r="D2" s="6" t="s">
         <x:v>23</x:v>
       </x:c>
-      <x:c r="E2" s="5" t="s">
+      <x:c r="E2" s="6" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="F2" s="5" t="s">
+      <x:c r="F2" s="6" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="G2" s="5" t="s">
+      <x:c r="G2" s="6" t="s">
         <x:v>26</x:v>
       </x:c>
-      <x:c r="H2" s="5" t="s">
+      <x:c r="H2" s="6" t="s">
         <x:v>27</x:v>
       </x:c>
-      <x:c r="I2" s="5" t="s">
+      <x:c r="I2" s="6" t="s">
         <x:v>28</x:v>
       </x:c>
-      <x:c r="J2" s="5" t="s">
+      <x:c r="J2" s="6" t="s">
         <x:v>29</x:v>
       </x:c>
-      <x:c r="K2" s="5" t="s">
+      <x:c r="K2" s="6" t="s">
         <x:v>30</x:v>
       </x:c>
-      <x:c r="L2" s="5" t="s">
+      <x:c r="L2" s="6" t="s">
         <x:v>31</x:v>
       </x:c>
-      <x:c r="M2" s="5" t="s">
+      <x:c r="M2" s="6" t="s">
         <x:v>32</x:v>
       </x:c>
-      <x:c r="N2" s="5" t="s">
+      <x:c r="N2" s="6" t="s">
         <x:v>33</x:v>
       </x:c>
-      <x:c r="O2" s="5" t="s">
+      <x:c r="O2" s="6" t="s">
         <x:v>34</x:v>
       </x:c>
-      <x:c r="P2" s="5" t="s">
+      <x:c r="P2" s="6" t="s">
         <x:v>35</x:v>
       </x:c>
-      <x:c r="Q2" s="5" t="s">
+      <x:c r="Q2" s="6" t="s">
         <x:v>36</x:v>
       </x:c>
-      <x:c r="R2" s="5" t="s">
+      <x:c r="R2" s="6" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="S2" s="5" t="s">
+      <x:c r="S2" s="6" t="s">
         <x:v>37</x:v>
       </x:c>
-      <x:c r="T2" s="5" t="s">
+      <x:c r="T2" s="6" t="s">
         <x:v>38</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A3" s="5" t="s"/>
-      <x:c r="B3" s="7" t="s"/>
-      <x:c r="C3" s="5" t="s"/>
-      <x:c r="D3" s="5" t="s"/>
-      <x:c r="E3" s="5" t="s"/>
-      <x:c r="F3" s="5" t="s"/>
-      <x:c r="G3" s="5" t="s"/>
-      <x:c r="H3" s="5" t="s"/>
-      <x:c r="I3" s="5" t="s"/>
-      <x:c r="J3" s="5" t="s"/>
-      <x:c r="K3" s="5" t="s"/>
-      <x:c r="L3" s="5" t="s"/>
-      <x:c r="M3" s="5" t="s"/>
-      <x:c r="N3" s="5" t="s"/>
-      <x:c r="O3" s="5" t="s"/>
-      <x:c r="P3" s="5" t="s"/>
-      <x:c r="Q3" s="5" t="s"/>
-      <x:c r="R3" s="5" t="s"/>
-      <x:c r="S3" s="5" t="s"/>
-      <x:c r="T3" s="5" t="s"/>
+      <x:c r="A3" s="6" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B3" s="7" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="C3" s="6" t="s">
+        <x:v>41</x:v>
+      </x:c>
+      <x:c r="D3" s="6" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="E3" s="6" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="F3" s="6" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="G3" s="6" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="H3" s="6" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="I3" s="6" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="J3" s="6" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="K3" s="6" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="L3" s="6" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="M3" s="6" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="N3" s="6" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="O3" s="6" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="P3" s="6" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="Q3" s="6" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="R3" s="6" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="S3" s="6" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="T3" s="6" t="s">
+        <x:v>38</x:v>
+      </x:c>
     </x:row>
     <x:row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A4" s="5" t="s"/>
-      <x:c r="B4" s="7" t="s"/>
-      <x:c r="C4" s="5" t="s"/>
-      <x:c r="D4" s="5" t="s"/>
-      <x:c r="E4" s="5" t="s"/>
-      <x:c r="F4" s="5" t="s"/>
-      <x:c r="G4" s="5" t="s"/>
-      <x:c r="H4" s="5" t="s"/>
-      <x:c r="I4" s="5" t="s"/>
-      <x:c r="J4" s="5" t="s"/>
-      <x:c r="K4" s="5" t="s"/>
-      <x:c r="L4" s="5" t="s"/>
-      <x:c r="M4" s="5" t="s"/>
-      <x:c r="N4" s="5" t="s"/>
-      <x:c r="O4" s="5" t="s"/>
-      <x:c r="P4" s="5" t="s"/>
-      <x:c r="Q4" s="5" t="s"/>
-      <x:c r="R4" s="5" t="s"/>
-      <x:c r="S4" s="5" t="s"/>
-      <x:c r="T4" s="5" t="s"/>
+      <x:c r="A4" s="6" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="B4" s="7" t="s">
+        <x:v>57</x:v>
+      </x:c>
+      <x:c r="C4" s="6" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="D4" s="6" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="E4" s="6" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="F4" s="6" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="G4" s="6" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="H4" s="6" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I4" s="6" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="J4" s="6" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="K4" s="6" t="s">
+        <x:v>65</x:v>
+      </x:c>
+      <x:c r="L4" s="6" t="s">
+        <x:v>66</x:v>
+      </x:c>
+      <x:c r="M4" s="6" t="s">
+        <x:v>67</x:v>
+      </x:c>
+      <x:c r="N4" s="6" t="s">
+        <x:v>68</x:v>
+      </x:c>
+      <x:c r="O4" s="6" t="s">
+        <x:v>69</x:v>
+      </x:c>
+      <x:c r="P4" s="6" t="s">
+        <x:v>70</x:v>
+      </x:c>
+      <x:c r="Q4" s="6" t="s">
+        <x:v>71</x:v>
+      </x:c>
+      <x:c r="R4" s="6" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="S4" s="6" t="s">
+        <x:v>56</x:v>
+      </x:c>
+      <x:c r="T4" s="6" t="s">
+        <x:v>38</x:v>
+      </x:c>
     </x:row>
     <x:row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A5" s="5" t="s"/>
+      <x:c r="A5" s="6" t="s"/>
       <x:c r="B5" s="7" t="s"/>
-      <x:c r="C5" s="5" t="s"/>
-      <x:c r="D5" s="5" t="s"/>
-      <x:c r="E5" s="5" t="s"/>
-      <x:c r="F5" s="5" t="s"/>
-      <x:c r="G5" s="5" t="s"/>
-      <x:c r="H5" s="5" t="s"/>
-      <x:c r="I5" s="5" t="s"/>
-      <x:c r="J5" s="5" t="s"/>
-      <x:c r="K5" s="5" t="s"/>
-      <x:c r="L5" s="5" t="s"/>
-      <x:c r="M5" s="5" t="s"/>
-      <x:c r="N5" s="5" t="s"/>
-      <x:c r="O5" s="5" t="s"/>
-      <x:c r="P5" s="5" t="s"/>
-      <x:c r="Q5" s="5" t="s"/>
-      <x:c r="R5" s="5" t="s"/>
-      <x:c r="S5" s="5" t="s"/>
-      <x:c r="T5" s="5" t="s"/>
+      <x:c r="C5" s="6" t="s"/>
+      <x:c r="D5" s="6" t="s"/>
+      <x:c r="E5" s="6" t="s"/>
+      <x:c r="F5" s="6" t="s"/>
+      <x:c r="G5" s="6" t="s"/>
+      <x:c r="H5" s="6" t="s"/>
+      <x:c r="I5" s="6" t="s"/>
+      <x:c r="J5" s="6" t="s"/>
+      <x:c r="K5" s="6" t="s"/>
+      <x:c r="L5" s="6" t="s"/>
+      <x:c r="M5" s="6" t="s"/>
+      <x:c r="N5" s="6" t="s"/>
+      <x:c r="O5" s="6" t="s"/>
+      <x:c r="P5" s="6" t="s"/>
+      <x:c r="Q5" s="6" t="s"/>
+      <x:c r="R5" s="6" t="s"/>
+      <x:c r="S5" s="6" t="s"/>
+      <x:c r="T5" s="6" t="s"/>
     </x:row>
     <x:row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A6" s="5" t="s"/>
-      <x:c r="B6" s="5" t="s"/>
-      <x:c r="C6" s="5" t="s"/>
-      <x:c r="D6" s="5" t="s"/>
-      <x:c r="E6" s="5" t="s"/>
-      <x:c r="F6" s="5" t="s"/>
-      <x:c r="G6" s="5" t="s"/>
-      <x:c r="H6" s="5" t="s"/>
-      <x:c r="I6" s="5" t="s"/>
-      <x:c r="J6" s="5" t="s"/>
-      <x:c r="K6" s="5" t="s"/>
-      <x:c r="L6" s="5" t="s"/>
-      <x:c r="M6" s="5" t="s"/>
-      <x:c r="N6" s="5" t="s"/>
-      <x:c r="O6" s="5" t="s"/>
-      <x:c r="P6" s="5" t="s"/>
-      <x:c r="Q6" s="5" t="s"/>
-      <x:c r="R6" s="5" t="s"/>
-      <x:c r="S6" s="5" t="s"/>
-      <x:c r="T6" s="5" t="s"/>
+      <x:c r="A6" s="6" t="s"/>
+      <x:c r="B6" s="6" t="s"/>
+      <x:c r="C6" s="6" t="s"/>
+      <x:c r="D6" s="6" t="s"/>
+      <x:c r="E6" s="6" t="s"/>
+      <x:c r="F6" s="6" t="s"/>
+      <x:c r="G6" s="6" t="s"/>
+      <x:c r="H6" s="6" t="s"/>
+      <x:c r="I6" s="6" t="s"/>
+      <x:c r="J6" s="6" t="s"/>
+      <x:c r="K6" s="6" t="s"/>
+      <x:c r="L6" s="6" t="s"/>
+      <x:c r="M6" s="6" t="s"/>
+      <x:c r="N6" s="6" t="s"/>
+      <x:c r="O6" s="6" t="s"/>
+      <x:c r="P6" s="6" t="s"/>
+      <x:c r="Q6" s="6" t="s"/>
+      <x:c r="R6" s="6" t="s"/>
+      <x:c r="S6" s="6" t="s"/>
+      <x:c r="T6" s="6" t="s"/>
     </x:row>
     <x:row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A7" s="5" t="s"/>
-      <x:c r="B7" s="5" t="s"/>
-      <x:c r="C7" s="5" t="s"/>
-      <x:c r="D7" s="5" t="s"/>
-      <x:c r="E7" s="5" t="s"/>
-      <x:c r="F7" s="5" t="s"/>
-      <x:c r="G7" s="5" t="s"/>
-      <x:c r="H7" s="5" t="s"/>
-      <x:c r="I7" s="5" t="s"/>
-      <x:c r="J7" s="5" t="s"/>
-      <x:c r="K7" s="5" t="s"/>
-      <x:c r="L7" s="5" t="s"/>
-      <x:c r="M7" s="5" t="s"/>
-      <x:c r="N7" s="5" t="s"/>
-      <x:c r="O7" s="5" t="s"/>
-      <x:c r="P7" s="5" t="s"/>
-      <x:c r="Q7" s="5" t="s"/>
-      <x:c r="R7" s="5" t="s"/>
-      <x:c r="S7" s="5" t="s"/>
-      <x:c r="T7" s="5" t="s"/>
+      <x:c r="B7" s="6" t="s"/>
     </x:row>
     <x:row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="B8" s="5" t="s"/>
+      <x:c r="B8" s="6" t="s"/>
     </x:row>
     <x:row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="B9" s="5" t="s"/>
+      <x:c r="B9" s="6" t="s"/>
     </x:row>
     <x:row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="B10" s="5" t="s"/>
+      <x:c r="B10" s="6" t="s"/>
     </x:row>
     <x:row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A11" s="5" t="s"/>
-      <x:c r="B11" s="5" t="s"/>
+      <x:c r="A11" s="6" t="s"/>
+      <x:c r="B11" s="6" t="s"/>
     </x:row>
     <x:row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <x:c r="A12" s="5" t="s"/>
-      <x:c r="B12" s="5" t="s"/>
-    </x:row>
+      <x:c r="A12" s="6" t="s"/>
+      <x:c r="B12" s="6" t="s"/>
+    </x:row>
+    <x:row r="16" spans="1:20"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>